<commit_message>
general fixes & top by country layout idea
</commit_message>
<xml_diff>
--- a/projetos/angular/app/Country.xlsx
+++ b/projetos/angular/app/Country.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpessia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiago Pessia\Documents\GitHub\portfolio\projetos\angular\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709CCB5D-F86A-4506-9875-A61D5D478C8F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12675" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12675" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Bolivia (Plurinational State of)</t>
   </si>
@@ -120,12 +121,57 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>KOREA, REPUBLIC OF</t>
+  </si>
+  <si>
+    <t>KOREA, DEMOCRATIC PEOPLE'S REPUBLIC OF</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>CAPE VERDE</t>
+  </si>
+  <si>
+    <t>HOLY SEE (VATICAN CITY STATE)</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>MICRONESIA, FEDERATED STATES OF</t>
+  </si>
+  <si>
+    <t>REUNION</t>
+  </si>
+  <si>
+    <t>VIRGIN ISLANDS, BRITISH</t>
+  </si>
+  <si>
+    <t>VIRGIN ISLANDS, U.S.</t>
+  </si>
+  <si>
+    <t>Cote D'ivoire</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Libyan Arab Jamahiriya</t>
+  </si>
+  <si>
+    <t>Saint Helena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,10 +216,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,11 +500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +514,7 @@
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
@@ -475,103 +522,142 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -582,15 +668,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -601,56 +690,62 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>